<commit_message>
Kompetencematrix.xlsx for KAS-qms-num updated
</commit_message>
<xml_diff>
--- a/autoqms/Content/KAS/Kompetencematrix.xlsx
+++ b/autoqms/Content/KAS/Kompetencematrix.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>Kørekort A</t>
   </si>
@@ -270,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -332,6 +332,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -828,7 +831,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1383,7 +1386,7 @@
       <c r="AG14" s="3"/>
     </row>
     <row r="15" spans="1:33" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="24" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -1421,13 +1424,11 @@
       <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
     </row>
-    <row r="16" spans="1:33" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -1461,11 +1462,11 @@
       <c r="AG16" s="3"/>
     </row>
     <row r="17" spans="1:33" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="24" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>

</xml_diff>